<commit_message>
Bug fixes toy example v2
</commit_message>
<xml_diff>
--- a/Data/FodstadDataSmall.xlsx
+++ b/Data/FodstadDataSmall.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berendmarkhorst/Library/Mobile Documents/com~apple~CloudDocs/PhD/READINESS/08 - Trondheim/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A11CCF9-68BE-984D-91CE-95BE409F0F40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD849C82-C161-8D4D-98AE-BD1177EFC036}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16060" activeTab="6" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26860" activeTab="4" xr2:uid="{D82E7092-1A4C-0041-9612-C431AA3B912B}"/>
   </bookViews>
   <sheets>
     <sheet name="Visualisation" sheetId="7" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="74">
   <si>
     <t>ID</t>
   </si>
@@ -72,12 +72,6 @@
     <t>Zeker</t>
   </si>
   <si>
-    <t>Production Capacity</t>
-  </si>
-  <si>
-    <t>Storage Capacity</t>
-  </si>
-  <si>
     <t>Shipper 1</t>
   </si>
   <si>
@@ -96,24 +90,12 @@
     <t>Demand</t>
   </si>
   <si>
-    <t>Gas</t>
-  </si>
-  <si>
-    <t>Hydrogen</t>
-  </si>
-  <si>
     <t>Vermoeden</t>
   </si>
   <si>
-    <t>Flow costs</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
-    <t>Production Costs</t>
-  </si>
-  <si>
     <t>Explanation</t>
   </si>
   <si>
@@ -123,9 +105,6 @@
     <t>NOK / MSm3</t>
   </si>
   <si>
-    <t>Entry Storage Costs</t>
-  </si>
-  <si>
     <t>MSm3</t>
   </si>
   <si>
@@ -144,24 +123,6 @@
     <t>Probability</t>
   </si>
   <si>
-    <t>Entry Costs Stage 1</t>
-  </si>
-  <si>
-    <t>Exit Costs Stage 1</t>
-  </si>
-  <si>
-    <t>Entry Costs Stage 2</t>
-  </si>
-  <si>
-    <t>Exit Costs Stage 2</t>
-  </si>
-  <si>
-    <t>Entry Costs Stage 3</t>
-  </si>
-  <si>
-    <t>Exit Costs Stage 3</t>
-  </si>
-  <si>
     <t>gas or mix</t>
   </si>
   <si>
@@ -177,18 +138,9 @@
     <t>Gamma</t>
   </si>
   <si>
-    <t>Hours</t>
-  </si>
-  <si>
     <t>Capacity</t>
   </si>
   <si>
-    <t>Entry Capacity</t>
-  </si>
-  <si>
-    <t>Exit Capacity</t>
-  </si>
-  <si>
     <t>Node Number</t>
   </si>
   <si>
@@ -220,13 +172,106 @@
   </si>
   <si>
     <t>Node 3</t>
+  </si>
+  <si>
+    <t>Number hours</t>
+  </si>
+  <si>
+    <t>Number markets</t>
+  </si>
+  <si>
+    <t>Number shippers</t>
+  </si>
+  <si>
+    <t>Production Capacity Gas</t>
+  </si>
+  <si>
+    <t>Entry Capacity Gas</t>
+  </si>
+  <si>
+    <t>Exit Capacity Gas</t>
+  </si>
+  <si>
+    <t>Production Costs Gas</t>
+  </si>
+  <si>
+    <t>Storage Capacity Gas</t>
+  </si>
+  <si>
+    <t>Entry Storage Costs Gas</t>
+  </si>
+  <si>
+    <t>Entry Costs Gas Stage 1</t>
+  </si>
+  <si>
+    <t>Exit Costs Gas Stage 1</t>
+  </si>
+  <si>
+    <t>Entry Costs Gas Stage 2</t>
+  </si>
+  <si>
+    <t>Exit Costs Gas Stage 2</t>
+  </si>
+  <si>
+    <t>Entry Costs Gas Stage 3</t>
+  </si>
+  <si>
+    <t>Exit Costs Gas Stage 3</t>
+  </si>
+  <si>
+    <t>Production Capacity Hydrogen</t>
+  </si>
+  <si>
+    <t>Entry Capacity Hydrogen</t>
+  </si>
+  <si>
+    <t>Exit Capacity Hydrogen</t>
+  </si>
+  <si>
+    <t>Production Costs Hydrogen</t>
+  </si>
+  <si>
+    <t>Storage Capacity Hydrogen</t>
+  </si>
+  <si>
+    <t>Entry Storage Costs Hydrogen</t>
+  </si>
+  <si>
+    <t>Entry Costs Hydrogen Stage 1</t>
+  </si>
+  <si>
+    <t>Exit Costs Hydrogen Stage 1</t>
+  </si>
+  <si>
+    <t>Entry Costs Hydrogen Stage 2</t>
+  </si>
+  <si>
+    <t>Exit Costs Hydrogen Stage 2</t>
+  </si>
+  <si>
+    <t>Entry Costs Hydrogen Stage 3</t>
+  </si>
+  <si>
+    <t>Exit Costs Hydrogen Stage 3</t>
+  </si>
+  <si>
+    <t>Flow costs Gas</t>
+  </si>
+  <si>
+    <t>Flow costs Hydrogen</t>
+  </si>
+  <si>
+    <t>X_coordinate</t>
+  </si>
+  <si>
+    <t>Y_coordinate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -250,13 +295,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -286,14 +324,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color rgb="FF202122"/>
       <name val="Calibri"/>
@@ -301,7 +331,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -316,11 +346,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -385,23 +410,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -409,22 +433,19 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="3" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -437,9 +458,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="3">
     <cellStyle name="Goed" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutraal" xfId="3" builtinId="28"/>
     <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -832,103 +852,103 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="68" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="str">
-        <f>Nodes!F3</f>
-        <v>Production Capacity</v>
+        <f>Nodes!H2</f>
+        <v>Production Capacity Gas</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="str">
-        <f>Nodes!I3</f>
-        <v>Production Costs</v>
+        <f>Nodes!K2</f>
+        <v>Production Costs Gas</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="str">
-        <f>Nodes!J3</f>
-        <v>Storage Capacity</v>
+        <f>Nodes!L2</f>
+        <v>Storage Capacity Gas</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C4" s="8"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="str">
-        <f>Nodes!K3</f>
-        <v>Entry Storage Costs</v>
+        <f>Nodes!M2</f>
+        <v>Entry Storage Costs Gas</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="str">
-        <f>Nodes!L3</f>
-        <v>Entry Costs Stage 1</v>
+        <f>Nodes!N2</f>
+        <v>Entry Costs Gas Stage 1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="str">
-        <f>Nodes!M3</f>
-        <v>Exit Costs Stage 1</v>
+        <f>Nodes!O2</f>
+        <v>Exit Costs Gas Stage 1</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="str">
-        <f>Arcs!G3</f>
-        <v>Flow costs</v>
+        <f>Arcs!G1</f>
+        <v>Flow costs Gas</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="str">
-        <f>Arcs!E3</f>
+        <f>Arcs!E1</f>
         <v>Capacity</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C9" s="8"/>
     </row>
     <row r="10" spans="1:3" ht="19" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="C10" s="1"/>
     </row>
@@ -939,529 +959,460 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA3F5746-A1B1-6F4F-9762-CACD4A91B5F2}">
-  <dimension ref="A1:AI6"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17.5" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" customWidth="1"/>
-    <col min="16" max="16" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.83203125" customWidth="1"/>
-    <col min="18" max="18" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="15" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="15" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="24" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="F1" s="14" t="str">
-        <f>Traders!B2</f>
-        <v>Shipper 1</v>
-      </c>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14" t="str">
-        <f>Traders!B3</f>
-        <v>Shipper 2</v>
-      </c>
-      <c r="Y1" s="14"/>
-      <c r="Z1" s="14"/>
-      <c r="AA1" s="14"/>
-      <c r="AB1" s="14"/>
-      <c r="AC1" s="14"/>
-      <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
-      <c r="AF1" s="14"/>
-      <c r="AG1" s="14"/>
-      <c r="AH1" s="14"/>
-      <c r="AI1" s="14"/>
-    </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A2" s="7"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="16" t="str">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="14" t="str">
         <f>Commodities!B2</f>
         <v>gas</v>
       </c>
-      <c r="G2" s="17"/>
-      <c r="H2" s="17"/>
-      <c r="I2" s="17"/>
-      <c r="J2" s="17"/>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="17"/>
-      <c r="O2" s="17"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="18"/>
-      <c r="R2" s="13" t="str">
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="13" t="str">
         <f>Commodities!B3</f>
         <v>hydrogen</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="13"/>
-      <c r="V2" s="13"/>
-      <c r="W2" s="13"/>
-      <c r="X2" s="15" t="str">
-        <f>Commodities!B2</f>
-        <v>gas</v>
-      </c>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="13" t="str">
-        <f>Commodities!B3</f>
-        <v>hydrogen</v>
-      </c>
-      <c r="AE2" s="13"/>
-      <c r="AF2" s="13"/>
-      <c r="AG2" s="13"/>
-      <c r="AH2" s="13"/>
-      <c r="AI2" s="13"/>
-    </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
+      <c r="U1" s="13"/>
+      <c r="V1" s="13"/>
+      <c r="W1" s="13"/>
+      <c r="X1" s="13"/>
+      <c r="Y1" s="13"/>
+      <c r="Z1" s="13"/>
+      <c r="AA1" s="13"/>
+      <c r="AB1" s="13"/>
+      <c r="AC1" s="13"/>
+      <c r="AD1" s="13"/>
+      <c r="AE1" s="13"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="4" t="s">
+      <c r="F2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="J3" s="5" t="s">
+      <c r="J2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="T2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="U2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="V2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="X2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z2" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA2" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC2" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD2" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="AE2" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="12">
+        <v>5</v>
+      </c>
+      <c r="I3" s="12">
         <v>10</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L3" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="N3" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="R3" s="6" t="str">
-        <f>F3</f>
-        <v>Production Capacity</v>
-      </c>
-      <c r="S3" s="6" t="str">
-        <f t="shared" ref="S3:W3" si="0">I3</f>
-        <v>Production Costs</v>
-      </c>
-      <c r="T3" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Storage Capacity</v>
-      </c>
-      <c r="U3" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Entry Storage Costs</v>
-      </c>
-      <c r="V3" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Entry Costs Stage 1</v>
-      </c>
-      <c r="W3" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>Exit Costs Stage 1</v>
-      </c>
-      <c r="X3" s="5" t="str">
-        <f t="shared" ref="X3:AI3" si="1">R3</f>
-        <v>Production Capacity</v>
-      </c>
-      <c r="Y3" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Production Costs</v>
-      </c>
-      <c r="Z3" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Storage Capacity</v>
-      </c>
-      <c r="AA3" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Entry Storage Costs</v>
-      </c>
-      <c r="AB3" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Entry Costs Stage 1</v>
-      </c>
-      <c r="AC3" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>Exit Costs Stage 1</v>
-      </c>
-      <c r="AD3" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Production Capacity</v>
-      </c>
-      <c r="AE3" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Production Costs</v>
-      </c>
-      <c r="AF3" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Storage Capacity</v>
-      </c>
-      <c r="AG3" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Entry Storage Costs</v>
-      </c>
-      <c r="AH3" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Entry Costs Stage 1</v>
-      </c>
-      <c r="AI3" s="6" t="str">
-        <f t="shared" si="1"/>
-        <v>Exit Costs Stage 1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
+      <c r="J3" s="12">
+        <v>0</v>
+      </c>
+      <c r="K3" s="2">
+        <v>1</v>
+      </c>
+      <c r="L3" s="2">
+        <v>10</v>
+      </c>
+      <c r="M3" s="2">
+        <v>0</v>
+      </c>
+      <c r="N3" s="2">
+        <v>1</v>
+      </c>
+      <c r="O3" s="2">
+        <v>1</v>
+      </c>
+      <c r="P3" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="2">
+        <v>3</v>
+      </c>
+      <c r="R3" s="2">
+        <v>5</v>
+      </c>
+      <c r="S3" s="2">
+        <v>5</v>
+      </c>
+      <c r="T3" s="3">
+        <v>0</v>
+      </c>
+      <c r="U3" s="3">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>0</v>
+      </c>
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD3" s="3">
+        <v>5</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C4" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0</v>
+      </c>
+      <c r="J4" s="12">
+        <v>10</v>
+      </c>
+      <c r="K4" s="2">
+        <v>1</v>
+      </c>
+      <c r="L4" s="2">
+        <v>10</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0</v>
+      </c>
+      <c r="N4" s="2">
+        <v>1</v>
+      </c>
+      <c r="O4" s="2">
+        <v>1</v>
+      </c>
+      <c r="P4" s="2">
+        <v>3</v>
+      </c>
+      <c r="Q4" s="2">
+        <v>3</v>
+      </c>
+      <c r="R4" s="2">
         <v>5</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="12">
+      <c r="S4" s="2">
         <v>5</v>
       </c>
-      <c r="G4" s="12">
+      <c r="T4" s="3">
+        <v>0</v>
+      </c>
+      <c r="U4" s="3">
+        <v>0</v>
+      </c>
+      <c r="V4" s="3">
+        <v>0</v>
+      </c>
+      <c r="W4" s="3">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>3</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>3</v>
+      </c>
+      <c r="AD4" s="3">
+        <v>5</v>
+      </c>
+      <c r="AE4" s="3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>1</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="12">
+        <v>5</v>
+      </c>
+      <c r="I5" s="12">
         <v>10</v>
       </c>
-      <c r="H4" s="12">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>1</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2">
+      <c r="J5" s="12">
+        <v>0</v>
+      </c>
+      <c r="K5" s="2">
+        <v>1</v>
+      </c>
+      <c r="L5" s="2">
+        <v>10</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="2">
+        <v>1</v>
+      </c>
+      <c r="P5" s="2">
         <v>3</v>
       </c>
-      <c r="O4" s="2">
+      <c r="Q5" s="2">
         <v>3</v>
       </c>
-      <c r="P4" s="2">
+      <c r="R5" s="2">
         <v>5</v>
       </c>
-      <c r="Q4" s="2">
+      <c r="S5" s="2">
         <v>5</v>
       </c>
-      <c r="R4" s="3">
-        <v>0</v>
-      </c>
-      <c r="S4" s="3">
-        <v>0</v>
-      </c>
-      <c r="T4" s="3">
-        <v>0</v>
-      </c>
-      <c r="U4" s="3">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3">
-        <v>0</v>
-      </c>
-      <c r="W4" s="3">
-        <v>0</v>
-      </c>
-      <c r="X4" s="2">
-        <f>R4</f>
-        <v>0</v>
-      </c>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
-      <c r="AA4" s="2"/>
-      <c r="AB4" s="2"/>
-      <c r="AC4" s="2"/>
-      <c r="AD4" s="3">
-        <f>X4</f>
-        <v>0</v>
-      </c>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
-    </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="1"/>
-      <c r="E5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="12">
-        <v>0</v>
-      </c>
-      <c r="G5" s="12">
-        <v>0</v>
-      </c>
-      <c r="H5" s="12">
-        <v>10</v>
-      </c>
-      <c r="I5" s="2">
-        <v>1</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>1</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
-      <c r="N5" s="2">
+      <c r="T5" s="3">
+        <v>0</v>
+      </c>
+      <c r="U5" s="3">
+        <v>0</v>
+      </c>
+      <c r="V5" s="3">
+        <v>0</v>
+      </c>
+      <c r="W5" s="3">
+        <v>0</v>
+      </c>
+      <c r="X5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="3">
         <v>3</v>
       </c>
-      <c r="O5" s="2">
+      <c r="AC5" s="3">
         <v>3</v>
       </c>
-      <c r="P5" s="2">
+      <c r="AD5" s="3">
         <v>5</v>
       </c>
-      <c r="Q5" s="2">
+      <c r="AE5" s="3">
         <v>5</v>
       </c>
-      <c r="R5" s="3">
-        <v>0</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0</v>
-      </c>
-      <c r="T5" s="3">
-        <v>0</v>
-      </c>
-      <c r="U5" s="3">
-        <v>0</v>
-      </c>
-      <c r="V5" s="3">
-        <v>0</v>
-      </c>
-      <c r="W5" s="3">
-        <v>0</v>
-      </c>
-      <c r="X5" s="2">
-        <f t="shared" ref="X5:X6" si="2">R5</f>
-        <v>0</v>
-      </c>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
-      <c r="AA5" s="2"/>
-      <c r="AB5" s="2"/>
-      <c r="AC5" s="2"/>
-      <c r="AD5" s="3">
-        <f t="shared" ref="AD5:AD6" si="3">X5</f>
-        <v>0</v>
-      </c>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
-    </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="1"/>
-      <c r="E6" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="12">
-        <v>5</v>
-      </c>
-      <c r="G6" s="12">
-        <v>10</v>
-      </c>
-      <c r="H6" s="12">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2">
-        <v>1</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0</v>
-      </c>
-      <c r="K6" s="2">
-        <v>0</v>
-      </c>
-      <c r="L6" s="2">
-        <v>1</v>
-      </c>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="N6" s="2">
-        <v>3</v>
-      </c>
-      <c r="O6" s="2">
-        <v>3</v>
-      </c>
-      <c r="P6" s="2">
-        <v>5</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>5</v>
-      </c>
-      <c r="R6" s="3">
-        <v>0</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0</v>
-      </c>
-      <c r="T6" s="3">
-        <v>0</v>
-      </c>
-      <c r="U6" s="3">
-        <v>0</v>
-      </c>
-      <c r="V6" s="3">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3">
-        <v>0</v>
-      </c>
-      <c r="X6" s="2">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
-      <c r="AA6" s="2"/>
-      <c r="AB6" s="2"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="3">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="AE6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="R2:W2"/>
-    <mergeCell ref="F1:W1"/>
-    <mergeCell ref="X1:AI1"/>
-    <mergeCell ref="X2:AC2"/>
-    <mergeCell ref="AD2:AI2"/>
-    <mergeCell ref="F2:Q2"/>
+  <mergeCells count="2">
+    <mergeCell ref="T1:AE1"/>
+    <mergeCell ref="H1:S1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1473,7 +1424,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1485,55 +1436,55 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="19">
-        <v>1</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+        <v>32</v>
+      </c>
+      <c r="B1" s="18">
+        <v>2</v>
+      </c>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="19">
-        <v>1</v>
-      </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
+        <v>25</v>
+      </c>
+      <c r="B2" s="18">
+        <v>1</v>
+      </c>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
-      <c r="B3" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
+      <c r="B3" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
       <c r="E3" s="13" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F3" s="13"/>
       <c r="G3" s="13"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E4" s="6" t="str">
         <f>B4</f>
@@ -1556,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2">
         <v>0</v>
@@ -1575,12 +1526,24 @@
       <c r="A6" s="1">
         <v>1</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
@@ -1827,7 +1790,7 @@
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B30">
         <f>SUM(B5:D5)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -1845,8 +1808,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7506CF-850A-ED42-956F-025E5A994524}">
   <dimension ref="A1:M31"/>
   <sheetViews>
-    <sheetView zoomScale="113" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="113" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1858,85 +1821,85 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="19">
-        <v>2</v>
-      </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19">
+        <v>32</v>
+      </c>
+      <c r="B1" s="18">
         <v>3</v>
       </c>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18">
+        <v>4</v>
+      </c>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B2" s="19">
+        <v>25</v>
+      </c>
+      <c r="B2" s="18">
         <v>0.5</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19">
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18">
         <v>0.5</v>
       </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B3" s="20">
-        <v>1</v>
-      </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="20">
-        <v>1</v>
-      </c>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
+        <v>33</v>
+      </c>
+      <c r="B3" s="19">
+        <v>3</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="19">
+        <v>3</v>
+      </c>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="20"/>
+      <c r="M3" s="20"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
-      <c r="B4" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
+      <c r="B4" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
       <c r="E4" s="13" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="F4" s="13"/>
       <c r="G4" s="13"/>
-      <c r="H4" s="15" t="str">
+      <c r="H4" s="17" t="str">
         <f>B4</f>
         <v>gas or mix</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
       <c r="K4" s="13" t="str">
         <f>E4</f>
         <v>pure hydrogen</v>
@@ -1946,16 +1909,16 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>56</v>
+        <v>40</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>58</v>
+        <v>42</v>
       </c>
       <c r="E5" s="6" t="str">
         <f>B5</f>
@@ -2002,7 +1965,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2">
         <v>0</v>
@@ -2020,7 +1983,7 @@
         <v>0</v>
       </c>
       <c r="I6" s="2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J6" s="2">
         <v>0</v>
@@ -2042,18 +2005,42 @@
       <c r="A7" s="1">
         <v>1</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>0</v>
+      </c>
+      <c r="H7" s="2">
+        <v>0</v>
+      </c>
+      <c r="I7" s="2">
+        <v>5</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="M7" s="3">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
@@ -2432,7 +2419,7 @@
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B31">
         <f>SUM(B6:D6)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2454,7 +2441,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D89E28-915C-F54C-B37A-2FAB20B0DB56}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
@@ -2470,12 +2457,12 @@
         <v>1</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -2483,15 +2470,15 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>0.25</v>
@@ -2499,15 +2486,15 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -2515,10 +2502,26 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B7">
         <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -2528,92 +2531,113 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2902688A-D2A3-854F-B341-C0BEC53AF991}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="150" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G1" s="14" t="str">
-        <f>Traders!B2</f>
-        <v>Shipper 1</v>
-      </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14" t="str">
-        <f>Traders!B3</f>
-        <v>Shipper 2</v>
-      </c>
-      <c r="J1" s="14"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="G2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="F3" s="4" t="s">
+      <c r="E1" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G1" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="1">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="2">
+        <v>1</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="E4" s="1">
         <v>10</v>
@@ -2627,70 +2651,8 @@
       <c r="H4" s="3">
         <v>0</v>
       </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
-        <v>2</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="E5" s="1">
-        <v>10</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" s="2">
-        <v>1</v>
-      </c>
-      <c r="H5" s="3">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>3</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E6" s="1">
-        <v>10</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="3">
-        <v>0</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2719,7 +2681,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2727,7 +2689,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -2758,7 +2720,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
@@ -2766,7 +2728,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>